<commit_message>
Iteration works fine, test will be processed
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UI programy\REFPefromProcess\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B71FC7A6-C0FA-411B-AD42-CD832A753B72}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02B26970-FD4A-4AE3-98C9-7E04A20CCC66}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31635" yWindow="2835" windowWidth="17280" windowHeight="8970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
   <si>
     <t>Name</t>
   </si>
@@ -137,10 +137,7 @@
     <t>ReportsDownloadPath</t>
   </si>
   <si>
-    <t xml:space="preserve">Data\Temp </t>
-  </si>
-  <si>
-    <t>Data\Temp\Result</t>
+    <t>Data\Temp\</t>
   </si>
 </sst>
 </file>
@@ -530,7 +527,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -627,7 +624,7 @@
         <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>